<commit_message>
Ruteo pcb V3 completo
</commit_message>
<xml_diff>
--- a/Hardware/pcb v3/bom/bom.xlsx
+++ b/Hardware/pcb v3/bom/bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="140">
   <si>
     <t>Qty</t>
   </si>
@@ -110,18 +110,6 @@
     <t>C12, C13</t>
   </si>
   <si>
-    <t>1200uF</t>
-  </si>
-  <si>
-    <t>CPOL-USUD-10X10</t>
-  </si>
-  <si>
-    <t>UD-10X10_NICHICON</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
     <t>POLARIZED CAPACITOR, American symbol</t>
   </si>
   <si>
@@ -299,15 +287,6 @@
     <t>478-1395-1-ND</t>
   </si>
   <si>
-    <t>United Chemi-Con</t>
-  </si>
-  <si>
-    <t>EMZJ100ADA122MJA0G</t>
-  </si>
-  <si>
-    <t>565-3654-1-ND</t>
-  </si>
-  <si>
     <t>490-10516-1-ND</t>
   </si>
   <si>
@@ -459,6 +438,12 @@
   </si>
   <si>
     <t>Precios digikey:</t>
+  </si>
+  <si>
+    <t>565-2075-1-ND</t>
+  </si>
+  <si>
+    <t>15x4</t>
   </si>
 </sst>
 </file>
@@ -466,7 +451,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -641,10 +626,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -963,11 +948,12 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
@@ -981,7 +967,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -999,13 +985,13 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>5</v>
@@ -1013,70 +999,70 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>B2*100</f>
-        <v>100</v>
+        <f>B2*4</f>
+        <v>4</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A26" si="0">B3*100</f>
-        <v>100</v>
+        <f t="shared" ref="A3:A26" si="0">B3*4</f>
+        <v>4</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
-        <v>600</v>
+        <v>24</v>
       </c>
       <c r="B4" s="4">
         <v>6</v>
@@ -1096,7 +1082,7 @@
       <c r="G4" s="8"/>
       <c r="H4" s="5"/>
       <c r="I4" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>15</v>
@@ -1105,40 +1091,30 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
         <v>2</v>
@@ -1158,7 +1134,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="9" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>15</v>
@@ -1167,7 +1143,7 @@
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
@@ -1187,7 +1163,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>15</v>
@@ -1196,13 +1172,13 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>8</v>
       </c>
       <c r="B8" s="4">
         <v>2</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>12</v>
@@ -1211,12 +1187,12 @@
         <v>13</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="6" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>15</v>
@@ -1225,7 +1201,7 @@
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -1245,7 +1221,7 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>15</v>
@@ -1254,145 +1230,145 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B11" s="4">
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>8</v>
       </c>
       <c r="B12" s="4">
         <v>2</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E12" s="5">
         <v>471511071</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="H12" s="8">
         <v>471511071</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B13" s="4">
         <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>10</v>
@@ -1400,16 +1376,16 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
@@ -1434,36 +1410,36 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="8" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>1400</v>
+        <v>56</v>
       </c>
       <c r="B17" s="4">
         <v>14</v>
@@ -1478,12 +1454,12 @@
         <v>24</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>25</v>
@@ -1492,13 +1468,13 @@
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>12</v>
       </c>
       <c r="B18" s="4">
         <v>3</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>23</v>
@@ -1507,12 +1483,12 @@
         <v>24</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>25</v>
@@ -1521,13 +1497,13 @@
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>23</v>
@@ -1536,256 +1512,259 @@
         <v>24</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="17" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>8</v>
       </c>
       <c r="B22" s="4">
         <v>2</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="J24" s="7"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="J25" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B26" s="11">
         <v>1</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="J26" s="15"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C29" s="18" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D29" s="19"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C30" s="4" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D30" s="20">
         <f>418.93/35</f>
         <v>11.969428571428571</v>
       </c>
+      <c r="E30" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C31" s="4" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D31" s="21">
         <v>22.26</v>
@@ -1804,7 +1783,7 @@
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34" s="4" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D34" s="20">
         <f>1009.48/100</f>
@@ -1813,7 +1792,7 @@
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D35" s="21">
         <v>19.52</v>
@@ -1832,7 +1811,7 @@
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" s="11" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D38" s="23">
         <f>7125.25/1000</f>

</xml_diff>